<commit_message>
Added Order And OrderCategory
</commit_message>
<xml_diff>
--- a/src/Data/Source/data.xlsx
+++ b/src/Data/Source/data.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
-    <sheet name="Department" sheetId="2" r:id="rId2"/>
-    <sheet name="Contacts" sheetId="3" r:id="rId3"/>
-    <sheet name="ISO Services" sheetId="5" r:id="rId4"/>
-    <sheet name="ISO Category" sheetId="4" r:id="rId5"/>
+    <sheet name="Orders" sheetId="6" r:id="rId2"/>
+    <sheet name="Department" sheetId="2" r:id="rId3"/>
+    <sheet name="Contacts" sheetId="3" r:id="rId4"/>
+    <sheet name="ISO Services" sheetId="5" r:id="rId5"/>
+    <sheet name="ISO Category" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
   <si>
     <t>Text</t>
   </si>
@@ -289,7 +290,37 @@
     <t>ЗАПОВЕДИ</t>
   </si>
   <si>
-    <t>/order</t>
+    <t>/orders</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Нарежда в периода 3 – 4.01.2017 функциите директор на дирекция УТ да се изпълняват от Г. Димова – гл. арх.</t>
+  </si>
+  <si>
+    <t>РД-01</t>
+  </si>
+  <si>
+    <t>Премества Пламен Стоев на позиция в дейност 623</t>
+  </si>
+  <si>
+    <t>Заместване от 04.01.-06.01.2017 г. на Х.Атанасова от М.Добрева</t>
+  </si>
+  <si>
+    <t>Заместване от 04.01-06.01.2017 г. на М.Кукова от Л.Станчева</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
   </si>
 </sst>
 </file>
@@ -390,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -407,6 +438,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -690,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,10 +945,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="3" max="3" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="153" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="8">
+        <v>42738</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="8">
+        <v>42738</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="8">
+        <v>42739</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="8">
+        <v>42739</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +1101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -1257,7 +1389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -1501,7 +1633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>

</xml_diff>